<commit_message>
change y axis to have free scaling
</commit_message>
<xml_diff>
--- a/StatTables.xlsx
+++ b/StatTables.xlsx
@@ -10,6 +10,10 @@
     <sheet name="Warm AFDW Boot" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="cool glm" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="warm glm" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Cool AFDW per day Boot" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Warm AFDW per day Boot" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="cool AFDW per day glm" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="warm  AFDW per day glm" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -930,4 +934,532 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="15.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="18.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="11.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="13.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.932833333333333</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.932833333333333</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.00248414115646259</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0119289186507937</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.08633333333333</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3.08633333333333</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.00578662131519274</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.054271587326907</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10.7585714285714</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10.7585714285714</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0313214285714312</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.147286458333333</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6.212875</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6.212875</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0318099702380951</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0651238945578228</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8.85225</v>
+      </c>
+      <c r="D6" t="n">
+        <v>8.85225</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0236548752834467</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.120829828042328</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5.329125</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5.329125</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0256150793650794</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0680006944444445</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="15.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="18.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="11.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="13.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="11.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="11.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7.62014285714286</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7.62014285714286</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0184600549471694</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.378997692439591</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.49325</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.49325</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0156740551845135</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0511373188405798</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.853125</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.853125</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0286426921583851</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.114610688405797</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>29.5645714285714</v>
+      </c>
+      <c r="D5" t="n">
+        <v>29.5645714285714</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0672725414078676</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.41082527173913</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="44.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="11.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="11.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-4.90581063627031</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.417417161113429</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-11.7527765825066</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.0000000000000150328762006684</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.44523150837728</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.568843704757533</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.29859992811126</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.000107048816386244</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2.25020039331424</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.552191000638357</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4.07503996029075</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.000211970319649157</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1.19651250974114</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.538883237804496</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.22035577617136</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0321243217145331</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-1.74559153702552</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.755260903814658</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-2.31124307932387</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0260543194564904</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-1.70399711413855</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.742799282158141</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-2.29402094895371</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0271187899854395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="44.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="11.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="11.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="11.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-1.79784627930817</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.477744116713901</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-3.76319920310986</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.000864300912356545</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-0.982380232379726</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.65417807359896</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1.50170155807143</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.145222728691909</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-1.62984016455064</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.65417807359896</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-2.49143196681001</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0194303213505482</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.96800201301227</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.925147503890755</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4.28904795864944</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.000219269141785231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>